<commit_message>
changed Nat and Gyebi assignment
</commit_message>
<xml_diff>
--- a/server/loginDataAccess.xlsx
+++ b/server/loginDataAccess.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\2024ICBT\server\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0053D4A1-35E7-45DE-81DB-1331F5B38F31}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BF66079-3928-4321-BB6D-294E4E068C75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="dqm_placement" sheetId="1" r:id="rId1"/>
@@ -1460,7 +1460,7 @@
   <dimension ref="A1:I23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="A28" sqref="A28:XFD28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1927,8 +1927,8 @@
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A16" s="10" t="s">
-        <v>6</v>
+      <c r="A16" s="4" t="s">
+        <v>12</v>
       </c>
       <c r="B16" s="4" t="s">
         <v>25</v>
@@ -1954,7 +1954,7 @@
         <v>336</v>
       </c>
       <c r="I16" s="5" t="s">
-        <v>323</v>
+        <v>329</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.3">
@@ -2184,11 +2184,10 @@
     <hyperlink ref="A14" r:id="rId5" xr:uid="{DE681AFC-66F8-415A-9C4F-04CF55F0A9FA}"/>
     <hyperlink ref="A3" r:id="rId6" xr:uid="{74C90144-6B29-4F24-9A0A-97908146FAA4}"/>
     <hyperlink ref="A2" r:id="rId7" xr:uid="{9DAE8955-5296-4A96-BE41-F0D4D89EED46}"/>
-    <hyperlink ref="A16" r:id="rId8" xr:uid="{0A86EA83-5372-4B24-857B-0197E66FA2F0}"/>
-    <hyperlink ref="A23" r:id="rId9" xr:uid="{A68EAAD3-3FA1-4D5D-AEF2-3BDF361FF021}"/>
+    <hyperlink ref="A23" r:id="rId8" xr:uid="{A68EAAD3-3FA1-4D5D-AEF2-3BDF361FF021}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId10"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId9"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
terry no  longer handles north east , only oti
</commit_message>
<xml_diff>
--- a/server/loginDataAccess.xlsx
+++ b/server/loginDataAccess.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\2024ICBT\server\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D870216A-CF86-4BC8-86E2-F29FF0B6EA75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D72C750C-53E5-41F7-A22D-E394DFF42303}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18,7 +18,7 @@
     <sheet name="districtCODES" sheetId="7" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">dqm_placement!$A$1:$I$23</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">dqm_placement!$A$1:$I$22</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="666" uniqueCount="340">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="661" uniqueCount="340">
   <si>
     <t>email</t>
   </si>
@@ -1460,10 +1460,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I24"/>
+  <dimension ref="A1:I23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+      <selection activeCell="A23" sqref="A23:XFD23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2029,7 +2029,7 @@
         <v>28</v>
       </c>
       <c r="D19" s="4">
-        <f>E19</f>
+        <f t="shared" ref="D19:D23" si="0">E19</f>
         <v>4</v>
       </c>
       <c r="E19" s="4">
@@ -2060,7 +2060,7 @@
         <v>36</v>
       </c>
       <c r="D20" s="4">
-        <f>E20</f>
+        <f t="shared" si="0"/>
         <v>12</v>
       </c>
       <c r="E20" s="4">
@@ -2091,7 +2091,7 @@
         <v>32</v>
       </c>
       <c r="D21" s="4">
-        <f>E21</f>
+        <f t="shared" si="0"/>
         <v>15</v>
       </c>
       <c r="E21" s="4">
@@ -2122,7 +2122,7 @@
         <v>33</v>
       </c>
       <c r="D22" s="4">
-        <f>E22</f>
+        <f t="shared" si="0"/>
         <v>11</v>
       </c>
       <c r="E22" s="4">
@@ -2143,28 +2143,28 @@
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A23" s="10" t="s">
-        <v>8</v>
+      <c r="A23" s="11" t="s">
+        <v>339</v>
       </c>
       <c r="B23" s="4" t="s">
         <v>25</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="D23" s="4">
-        <f>E23</f>
-        <v>14</v>
+        <f t="shared" si="0"/>
+        <v>11</v>
       </c>
       <c r="E23" s="4">
         <f>VLOOKUP(C23,regionCODES!A:B,2,FALSE)</f>
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="F23" s="4">
-        <v>17</v>
+        <v>1</v>
       </c>
       <c r="G23" s="4">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="H23" s="4" t="s">
         <v>336</v>
@@ -2173,39 +2173,8 @@
         <v>330</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A24" s="11" t="s">
-        <v>339</v>
-      </c>
-      <c r="B24" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="C24" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="D24" s="4">
-        <f>E24</f>
-        <v>11</v>
-      </c>
-      <c r="E24" s="4">
-        <f>VLOOKUP(C24,regionCODES!A:B,2,FALSE)</f>
-        <v>11</v>
-      </c>
-      <c r="F24" s="4">
-        <v>1</v>
-      </c>
-      <c r="G24" s="4">
-        <v>13</v>
-      </c>
-      <c r="H24" s="4" t="s">
-        <v>336</v>
-      </c>
-      <c r="I24" s="5" t="s">
-        <v>330</v>
-      </c>
-    </row>
   </sheetData>
-  <autoFilter ref="A1:I23" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:I22" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <hyperlinks>
     <hyperlink ref="A17" r:id="rId1" xr:uid="{D626F59B-8E50-44E9-AC4C-8F2EA6B22CDC}"/>
     <hyperlink ref="A15" r:id="rId2" xr:uid="{740B8960-B9E1-4EBE-9BE7-4237D685F812}"/>
@@ -2214,11 +2183,10 @@
     <hyperlink ref="A14" r:id="rId5" xr:uid="{DE681AFC-66F8-415A-9C4F-04CF55F0A9FA}"/>
     <hyperlink ref="A3" r:id="rId6" xr:uid="{74C90144-6B29-4F24-9A0A-97908146FAA4}"/>
     <hyperlink ref="A2" r:id="rId7" xr:uid="{9DAE8955-5296-4A96-BE41-F0D4D89EED46}"/>
-    <hyperlink ref="A23" r:id="rId8" xr:uid="{A68EAAD3-3FA1-4D5D-AEF2-3BDF361FF021}"/>
-    <hyperlink ref="A24" r:id="rId9" xr:uid="{6B956567-910C-410F-9E7C-A90F6AE5440F}"/>
+    <hyperlink ref="A23" r:id="rId8" xr:uid="{6B956567-910C-410F-9E7C-A90F6AE5440F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId10"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId9"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
first serve of Filtering & Manual Reject 20241124
</commit_message>
<xml_diff>
--- a/server/loginDataAccess.xlsx
+++ b/server/loginDataAccess.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\2024ICBT\server\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D72C750C-53E5-41F7-A22D-E394DFF42303}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BC50640-4D36-4C2E-BDB3-D84B060090F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="661" uniqueCount="340">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="666" uniqueCount="341">
   <si>
     <t>email</t>
   </si>
@@ -1059,13 +1059,16 @@
   </si>
   <si>
     <t>andosty@gmail.com</t>
+  </si>
+  <si>
+    <t>andosty</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1115,8 +1118,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1132,6 +1143,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1152,7 +1169,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyFill="1"/>
@@ -1176,6 +1193,11 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1460,10 +1482,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I23"/>
+  <dimension ref="A1:I24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23:XFD23"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="I24" sqref="I24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2143,34 +2165,65 @@
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A23" s="11" t="s">
+      <c r="A23" s="15" t="s">
         <v>339</v>
       </c>
-      <c r="B23" s="4" t="s">
+      <c r="B23" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="C23" s="4" t="s">
+      <c r="C23" s="16" t="s">
         <v>33</v>
       </c>
-      <c r="D23" s="4">
+      <c r="D23" s="16">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="E23" s="4">
+      <c r="E23" s="16">
         <f>VLOOKUP(C23,regionCODES!A:B,2,FALSE)</f>
         <v>11</v>
       </c>
-      <c r="F23" s="4">
+      <c r="F23" s="16">
+        <v>4</v>
+      </c>
+      <c r="G23" s="16">
+        <v>8</v>
+      </c>
+      <c r="H23" s="16" t="s">
+        <v>336</v>
+      </c>
+      <c r="I23" s="17" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A24" s="15" t="s">
+        <v>339</v>
+      </c>
+      <c r="B24" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="C24" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="D24" s="16">
+        <f>E24</f>
+        <v>7</v>
+      </c>
+      <c r="E24" s="16">
+        <f>VLOOKUP(C24,regionCODES!A:B,2,FALSE)</f>
+        <v>7</v>
+      </c>
+      <c r="F24" s="16">
         <v>1</v>
       </c>
-      <c r="G23" s="4">
-        <v>13</v>
-      </c>
-      <c r="H23" s="4" t="s">
+      <c r="G24" s="16">
+        <v>5</v>
+      </c>
+      <c r="H24" s="16" t="s">
         <v>336</v>
       </c>
-      <c r="I23" s="5" t="s">
-        <v>330</v>
+      <c r="I24" s="17" t="s">
+        <v>340</v>
       </c>
     </row>
   </sheetData>
@@ -2184,9 +2237,10 @@
     <hyperlink ref="A3" r:id="rId6" xr:uid="{74C90144-6B29-4F24-9A0A-97908146FAA4}"/>
     <hyperlink ref="A2" r:id="rId7" xr:uid="{9DAE8955-5296-4A96-BE41-F0D4D89EED46}"/>
     <hyperlink ref="A23" r:id="rId8" xr:uid="{6B956567-910C-410F-9E7C-A90F6AE5440F}"/>
+    <hyperlink ref="A24" r:id="rId9" xr:uid="{B03A16A3-DC35-4DB2-96F3-94E8B885E018}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId9"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId10"/>
 </worksheet>
 </file>
 

</xml_diff>